<commit_message>
Topic added to tracker
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -63,9 +63,6 @@
     <t>BOOTSTRAP4</t>
   </si>
   <si>
-    <t>To Create mock page of Amazon.in(only homepage)</t>
-  </si>
-  <si>
     <t>TASK(HTML/CSS)</t>
   </si>
   <si>
@@ -73,6 +70,12 @@
   </si>
   <si>
     <t>Basics,Libraries,Methods.</t>
+  </si>
+  <si>
+    <t>To Create template of Amazon.in(only homepage)</t>
+  </si>
+  <si>
+    <t>Variables,operators,String Interpolation,Control Flow,Functions,</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -595,10 +598,10 @@
         <v>43318</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -606,10 +609,10 @@
         <v>43319</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -617,10 +620,21 @@
         <v>43320</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>18</v>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4">
+        <v>43321</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
python basics completed( functions and data structures )
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>Variables,operators,String Interpolation,Control Flow,Functions.</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>The Interpreter, And its Environment, Introducton to Python, Data Types, Operators</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lists, Tuples,Sets, Dictionaries, Compound data structures, and their Methods,</t>
+  </si>
+  <si>
+    <t>Control Flow tools, functions</t>
   </si>
 </sst>
 </file>
@@ -491,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -635,6 +647,39 @@
       </c>
       <c r="C12" s="7" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4">
+        <v>43322</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4">
+        <v>43323</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4">
+        <v>43324</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
traker updated (python entries made)
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Control Flow tools, functions</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>tasks on lists,tuples,sets,dictionaries,methods etc.</t>
   </si>
 </sst>
 </file>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -680,6 +686,17 @@
       </c>
       <c r="C15" s="7" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4">
+        <v>43325</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tracker updated And Python Task added
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -87,13 +87,16 @@
     <t xml:space="preserve"> Lists, Tuples,Sets, Dictionaries, Compound data structures, and their Methods,</t>
   </si>
   <si>
-    <t>Control Flow tools, functions</t>
-  </si>
-  <si>
     <t>python</t>
   </si>
   <si>
-    <t>tasks on lists,tuples,sets,dictionaries,methods etc.</t>
+    <t>pyhton</t>
+  </si>
+  <si>
+    <t>Control Flow tools, functions,function args,</t>
+  </si>
+  <si>
+    <t>tasks on lists,tuples,sets,dictionaries,methods ,function args,etc.</t>
   </si>
 </sst>
 </file>
@@ -509,9 +512,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -685,7 +688,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -693,10 +696,18 @@
         <v>43325</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4">
+        <v>43326</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
python Tasks Added and tracker updated
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -90,13 +90,13 @@
     <t>python</t>
   </si>
   <si>
-    <t>pyhton</t>
-  </si>
-  <si>
     <t>Control Flow tools, functions,function args,</t>
   </si>
   <si>
     <t>tasks on lists,tuples,sets,dictionaries,methods ,function args,etc.</t>
+  </si>
+  <si>
+    <t>Hankerank tasks on python</t>
   </si>
 </sst>
 </file>
@@ -512,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -688,7 +688,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -699,15 +699,40 @@
         <v>23</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>43326</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4">
+        <v>43327</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4">
+        <v>43328</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Python weekend tasks added
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Hankerank tasks on python</t>
+  </si>
+  <si>
+    <t>tasks:count word occurrences(case sensitive) and count word occurrences(case insensitive</t>
+  </si>
+  <si>
+    <t>tasks: Extract links from a webpage</t>
   </si>
 </sst>
 </file>
@@ -512,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -733,6 +739,39 @@
       </c>
       <c r="C19" s="7" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4">
+        <v>43329</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4">
+        <v>43330</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4">
+        <v>43331</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
python tasks and tracker updated
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -96,13 +96,28 @@
     <t>tasks on lists,tuples,sets,dictionaries,methods ,function args,etc.</t>
   </si>
   <si>
-    <t>Hankerank tasks on python</t>
-  </si>
-  <si>
     <t>tasks:count word occurrences(case sensitive) and count word occurrences(case insensitive</t>
   </si>
   <si>
-    <t>tasks: Extract links from a webpage</t>
+    <t>Hankerank tasks on python(intro)</t>
+  </si>
+  <si>
+    <t>Hankerank tasks on python(basic data types)</t>
+  </si>
+  <si>
+    <t>Hankerank tasks on python(strings)</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>Eid Celebration</t>
+  </si>
+  <si>
+    <t>tasks: Extract links from a webpage and Files I/O</t>
+  </si>
+  <si>
+    <t>Hankerank tasks on python(strings) and Exceptions</t>
   </si>
 </sst>
 </file>
@@ -518,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -716,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -727,7 +742,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -738,7 +753,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -749,7 +764,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -760,7 +775,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -771,7 +786,84 @@
         <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4">
+        <v>43332</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4">
+        <v>43333</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4">
+        <v>43334</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="4">
+        <v>43335</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4">
+        <v>43336</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4">
+        <v>43337</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="4">
+        <v>43338</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>